<commit_message>
Added write Learned if learn word
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -2588,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C499"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="E371" sqref="E371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Addet congratulations if + check button
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -1134,9 +1134,6 @@
     <t>goal</t>
   </si>
   <si>
-    <t>No learned</t>
-  </si>
-  <si>
     <t>способный</t>
   </si>
   <si>
@@ -2257,6 +2254,9 @@
   </si>
   <si>
     <t>хочет</t>
+  </si>
+  <si>
+    <t>Learned</t>
   </si>
 </sst>
 </file>
@@ -2589,7 +2589,7 @@
   <dimension ref="A1:C499"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
-      <selection activeCell="E371" sqref="E371"/>
+      <selection activeCell="C1" sqref="C1:C378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,7 +2608,7 @@
         <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>203</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2627,10 +2627,10 @@
         <v>145</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,10 +2638,10 @@
         <v>262</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,10 +2649,10 @@
         <v>195</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,10 +2660,10 @@
         <v>336</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,10 +2671,10 @@
         <v>330</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,10 +2682,10 @@
         <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2693,21 +2693,21 @@
         <v>352</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2715,21 +2715,21 @@
         <v>259</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2737,10 +2737,10 @@
         <v>187</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2748,10 +2748,10 @@
         <v>264</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2759,10 +2759,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,10 +2770,10 @@
         <v>353</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2781,10 +2781,10 @@
         <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2792,10 +2792,10 @@
         <v>141</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2803,10 +2803,10 @@
         <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2814,21 +2814,21 @@
         <v>241</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>125</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2847,10 +2847,10 @@
         <v>217</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2858,10 +2858,10 @@
         <v>252</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2869,10 +2869,10 @@
         <v>266</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2880,10 +2880,10 @@
         <v>286</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2891,10 +2891,10 @@
         <v>295</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2902,32 +2902,32 @@
         <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2935,10 +2935,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2946,21 +2946,21 @@
         <v>249</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,10 +2968,10 @@
         <v>337</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2979,10 +2979,10 @@
         <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2990,10 +2990,10 @@
         <v>91</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3001,10 +3001,10 @@
         <v>345</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3012,10 +3012,10 @@
         <v>273</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3023,10 +3023,10 @@
         <v>237</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3034,10 +3034,10 @@
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3045,10 +3045,10 @@
         <v>263</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3056,10 +3056,10 @@
         <v>287</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3067,10 +3067,10 @@
         <v>342</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3078,10 +3078,10 @@
         <v>207</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3089,10 +3089,10 @@
         <v>169</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3100,10 +3100,10 @@
         <v>311</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3111,10 +3111,10 @@
         <v>221</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3122,10 +3122,10 @@
         <v>192</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3133,10 +3133,10 @@
         <v>233</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3144,10 +3144,10 @@
         <v>354</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3155,10 +3155,10 @@
         <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
         <v>118</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3177,10 +3177,10 @@
         <v>173</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3188,21 +3188,21 @@
         <v>240</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3210,10 +3210,10 @@
         <v>15</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3221,21 +3221,21 @@
         <v>212</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,10 +3243,10 @@
         <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3254,10 +3254,10 @@
         <v>327</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3265,10 +3265,10 @@
         <v>355</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3276,10 +3276,10 @@
         <v>228</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3287,10 +3287,10 @@
         <v>89</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3298,10 +3298,10 @@
         <v>341</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3309,10 +3309,10 @@
         <v>300</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3320,10 +3320,10 @@
         <v>314</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3331,10 +3331,10 @@
         <v>235</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3342,10 +3342,10 @@
         <v>226</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3353,10 +3353,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3364,10 +3364,10 @@
         <v>175</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3375,10 +3375,10 @@
         <v>166</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3386,10 +3386,10 @@
         <v>87</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3397,10 +3397,10 @@
         <v>210</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3408,10 +3408,10 @@
         <v>146</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3419,10 +3419,10 @@
         <v>223</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3430,10 +3430,10 @@
         <v>356</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3441,10 +3441,10 @@
         <v>147</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3452,21 +3452,21 @@
         <v>30</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3474,10 +3474,10 @@
         <v>257</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -3485,21 +3485,21 @@
         <v>77</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3507,10 +3507,10 @@
         <v>167</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3518,21 +3518,21 @@
         <v>177</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3540,10 +3540,10 @@
         <v>254</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3554,7 +3554,7 @@
         <v>109</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3562,10 +3562,10 @@
         <v>246</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3573,10 +3573,10 @@
         <v>272</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3584,10 +3584,10 @@
         <v>357</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3595,10 +3595,10 @@
         <v>358</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3606,10 +3606,10 @@
         <v>26</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3617,10 +3617,10 @@
         <v>204</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3628,10 +3628,10 @@
         <v>24</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3639,10 +3639,10 @@
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3650,10 +3650,10 @@
         <v>43</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3661,10 +3661,10 @@
         <v>211</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3672,10 +3672,10 @@
         <v>183</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3683,10 +3683,10 @@
         <v>359</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3694,21 +3694,21 @@
         <v>239</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3716,10 +3716,10 @@
         <v>303</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3727,10 +3727,10 @@
         <v>152</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3738,10 +3738,10 @@
         <v>305</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3749,10 +3749,10 @@
         <v>291</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3760,21 +3760,21 @@
         <v>144</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3782,10 +3782,10 @@
         <v>318</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3793,21 +3793,21 @@
         <v>227</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3815,10 +3815,10 @@
         <v>158</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3826,10 +3826,10 @@
         <v>58</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3840,7 +3840,7 @@
         <v>116</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3848,10 +3848,10 @@
         <v>40</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3859,10 +3859,10 @@
         <v>142</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3870,10 +3870,10 @@
         <v>50</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3881,10 +3881,10 @@
         <v>255</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3892,10 +3892,10 @@
         <v>319</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3903,10 +3903,10 @@
         <v>220</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3917,7 +3917,7 @@
         <v>117</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3925,10 +3925,10 @@
         <v>335</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3936,10 +3936,10 @@
         <v>71</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3947,10 +3947,10 @@
         <v>258</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3958,10 +3958,10 @@
         <v>340</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3969,10 +3969,10 @@
         <v>3</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3980,32 +3980,32 @@
         <v>18</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4013,10 +4013,10 @@
         <v>198</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4024,10 +4024,10 @@
         <v>68</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -4038,7 +4038,7 @@
         <v>113</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4046,10 +4046,10 @@
         <v>164</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4057,10 +4057,10 @@
         <v>343</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -4068,10 +4068,10 @@
         <v>360</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -4079,10 +4079,10 @@
         <v>290</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -4090,10 +4090,10 @@
         <v>136</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -4101,10 +4101,10 @@
         <v>370</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4112,10 +4112,10 @@
         <v>55</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -4123,10 +4123,10 @@
         <v>95</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -4134,10 +4134,10 @@
         <v>299</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -4145,10 +4145,10 @@
         <v>66</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4156,10 +4156,10 @@
         <v>234</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4167,21 +4167,21 @@
         <v>52</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4189,10 +4189,10 @@
         <v>256</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -4200,10 +4200,10 @@
         <v>184</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4211,10 +4211,10 @@
         <v>156</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
         <v>120</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4233,10 +4233,10 @@
         <v>196</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -4244,10 +4244,10 @@
         <v>201</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4258,7 +4258,7 @@
         <v>123</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -4266,10 +4266,10 @@
         <v>20</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4277,10 +4277,10 @@
         <v>133</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -4288,10 +4288,10 @@
         <v>248</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4299,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4310,10 +4310,10 @@
         <v>275</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>243</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4332,10 +4332,10 @@
         <v>285</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -4343,10 +4343,10 @@
         <v>361</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4354,21 +4354,21 @@
         <v>31</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4376,10 +4376,10 @@
         <v>250</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4387,10 +4387,10 @@
         <v>244</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4398,10 +4398,10 @@
         <v>362</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -4409,10 +4409,10 @@
         <v>185</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -4420,43 +4420,43 @@
         <v>86</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -4467,7 +4467,7 @@
         <v>119</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -4475,10 +4475,10 @@
         <v>306</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -4486,21 +4486,21 @@
         <v>199</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -4508,10 +4508,10 @@
         <v>72</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -4519,10 +4519,10 @@
         <v>294</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -4530,10 +4530,10 @@
         <v>267</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -4541,10 +4541,10 @@
         <v>189</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -4552,10 +4552,10 @@
         <v>197</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -4563,10 +4563,10 @@
         <v>139</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -4574,10 +4574,10 @@
         <v>283</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -4585,10 +4585,10 @@
         <v>347</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -4596,10 +4596,10 @@
         <v>218</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -4607,21 +4607,21 @@
         <v>253</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -4629,10 +4629,10 @@
         <v>344</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -4640,10 +4640,10 @@
         <v>363</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -4651,10 +4651,10 @@
         <v>364</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -4662,10 +4662,10 @@
         <v>230</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -4673,10 +4673,10 @@
         <v>2</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -4684,10 +4684,10 @@
         <v>251</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -4695,10 +4695,10 @@
         <v>261</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -4706,10 +4706,10 @@
         <v>326</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -4717,10 +4717,10 @@
         <v>296</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -4728,10 +4728,10 @@
         <v>170</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -4739,10 +4739,10 @@
         <v>59</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -4750,21 +4750,21 @@
         <v>331</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -4772,10 +4772,10 @@
         <v>313</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -4783,10 +4783,10 @@
         <v>317</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -4794,10 +4794,10 @@
         <v>132</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -4805,10 +4805,10 @@
         <v>194</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -4816,10 +4816,10 @@
         <v>332</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -4827,10 +4827,10 @@
         <v>346</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4838,10 +4838,10 @@
         <v>56</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>128</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -4860,10 +4860,10 @@
         <v>302</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -4871,10 +4871,10 @@
         <v>165</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -4882,21 +4882,21 @@
         <v>310</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4904,10 +4904,10 @@
         <v>260</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -4915,10 +4915,10 @@
         <v>278</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -4926,21 +4926,21 @@
         <v>157</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -4948,10 +4948,10 @@
         <v>222</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -4962,7 +4962,7 @@
         <v>100</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -4970,10 +4970,10 @@
         <v>148</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -4981,10 +4981,10 @@
         <v>176</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -4992,10 +4992,10 @@
         <v>163</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -5003,10 +5003,10 @@
         <v>365</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -5014,10 +5014,10 @@
         <v>225</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -5025,10 +5025,10 @@
         <v>186</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -5036,21 +5036,21 @@
         <v>5</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -5058,10 +5058,10 @@
         <v>46</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -5069,10 +5069,10 @@
         <v>339</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -5080,10 +5080,10 @@
         <v>57</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -5091,10 +5091,10 @@
         <v>78</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -5102,10 +5102,10 @@
         <v>22</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -5113,10 +5113,10 @@
         <v>270</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -5124,10 +5124,10 @@
         <v>333</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -5135,10 +5135,10 @@
         <v>231</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -5146,10 +5146,10 @@
         <v>232</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -5157,10 +5157,10 @@
         <v>366</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -5168,10 +5168,10 @@
         <v>236</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -5179,10 +5179,10 @@
         <v>320</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -5190,10 +5190,10 @@
         <v>174</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -5201,10 +5201,10 @@
         <v>279</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -5212,10 +5212,10 @@
         <v>242</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -5223,21 +5223,21 @@
         <v>229</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -5245,10 +5245,10 @@
         <v>367</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -5256,10 +5256,10 @@
         <v>323</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -5267,10 +5267,10 @@
         <v>42</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -5278,10 +5278,10 @@
         <v>368</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -5289,10 +5289,10 @@
         <v>219</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -5300,10 +5300,10 @@
         <v>209</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -5311,10 +5311,10 @@
         <v>324</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -5322,10 +5322,10 @@
         <v>63</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -5333,10 +5333,10 @@
         <v>325</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -5344,10 +5344,10 @@
         <v>149</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -5358,7 +5358,7 @@
         <v>107</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -5366,10 +5366,10 @@
         <v>224</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -5377,10 +5377,10 @@
         <v>32</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -5388,10 +5388,10 @@
         <v>328</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -5399,10 +5399,10 @@
         <v>304</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -5410,10 +5410,10 @@
         <v>208</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -5421,10 +5421,10 @@
         <v>322</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -5432,10 +5432,10 @@
         <v>190</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -5443,10 +5443,10 @@
         <v>280</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -5454,10 +5454,10 @@
         <v>216</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -5465,10 +5465,10 @@
         <v>131</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -5476,10 +5476,10 @@
         <v>297</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -5487,10 +5487,10 @@
         <v>274</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -5501,7 +5501,7 @@
         <v>105</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -5509,10 +5509,10 @@
         <v>135</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -5520,10 +5520,10 @@
         <v>188</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -5531,10 +5531,10 @@
         <v>292</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -5542,10 +5542,10 @@
         <v>154</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -5553,10 +5553,10 @@
         <v>172</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -5564,21 +5564,21 @@
         <v>36</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -5586,10 +5586,10 @@
         <v>307</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -5597,10 +5597,10 @@
         <v>238</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -5608,10 +5608,10 @@
         <v>329</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -5619,10 +5619,10 @@
         <v>277</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -5630,10 +5630,10 @@
         <v>206</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -5641,10 +5641,10 @@
         <v>181</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -5652,10 +5652,10 @@
         <v>284</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -5663,10 +5663,10 @@
         <v>14</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -5674,21 +5674,21 @@
         <v>191</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -5696,10 +5696,10 @@
         <v>288</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -5707,10 +5707,10 @@
         <v>96</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -5718,21 +5718,21 @@
         <v>245</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -5740,10 +5740,10 @@
         <v>161</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -5751,10 +5751,10 @@
         <v>202</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -5762,10 +5762,10 @@
         <v>271</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -5773,10 +5773,10 @@
         <v>160</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -5784,10 +5784,10 @@
         <v>193</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -5798,7 +5798,7 @@
         <v>122</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -5806,21 +5806,21 @@
         <v>19</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -5828,10 +5828,10 @@
         <v>179</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -5839,10 +5839,10 @@
         <v>338</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -5850,10 +5850,10 @@
         <v>214</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -5861,10 +5861,10 @@
         <v>214</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -5872,21 +5872,21 @@
         <v>289</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -5894,10 +5894,10 @@
         <v>70</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -5905,10 +5905,10 @@
         <v>205</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -5916,10 +5916,10 @@
         <v>276</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -5927,10 +5927,10 @@
         <v>137</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -5938,10 +5938,10 @@
         <v>312</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -5949,10 +5949,10 @@
         <v>350</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -5960,10 +5960,10 @@
         <v>351</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -5971,10 +5971,10 @@
         <v>334</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -5982,10 +5982,10 @@
         <v>282</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -5993,21 +5993,21 @@
         <v>34</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -6015,10 +6015,10 @@
         <v>182</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -6026,10 +6026,10 @@
         <v>269</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -6037,10 +6037,10 @@
         <v>143</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -6048,10 +6048,10 @@
         <v>268</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -6059,10 +6059,10 @@
         <v>29</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -6070,10 +6070,10 @@
         <v>293</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -6081,10 +6081,10 @@
         <v>84</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -6095,7 +6095,7 @@
         <v>106</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -6106,7 +6106,7 @@
         <v>104</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -6117,7 +6117,7 @@
         <v>108</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -6125,10 +6125,10 @@
         <v>88</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -6136,10 +6136,10 @@
         <v>150</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -6150,7 +6150,7 @@
         <v>112</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -6158,10 +6158,10 @@
         <v>47</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -6169,10 +6169,10 @@
         <v>27</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -6180,10 +6180,10 @@
         <v>0</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -6194,7 +6194,7 @@
         <v>114</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -6202,10 +6202,10 @@
         <v>80</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -6213,10 +6213,10 @@
         <v>41</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -6224,10 +6224,10 @@
         <v>94</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -6238,7 +6238,7 @@
         <v>124</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -6246,10 +6246,10 @@
         <v>4</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
@@ -6260,7 +6260,7 @@
         <v>103</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -6268,10 +6268,10 @@
         <v>79</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -6279,10 +6279,10 @@
         <v>7</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -6290,10 +6290,10 @@
         <v>60</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -6304,7 +6304,7 @@
         <v>115</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -6312,10 +6312,10 @@
         <v>49</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -6326,7 +6326,7 @@
         <v>101</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -6334,10 +6334,10 @@
         <v>17</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
@@ -6348,7 +6348,7 @@
         <v>107</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -6359,7 +6359,7 @@
         <v>110</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -6370,7 +6370,7 @@
         <v>126</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
@@ -6381,7 +6381,7 @@
         <v>102</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -6389,10 +6389,10 @@
         <v>53</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -6400,10 +6400,10 @@
         <v>33</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -6411,10 +6411,10 @@
         <v>308</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -6422,10 +6422,10 @@
         <v>349</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -6436,7 +6436,7 @@
         <v>127</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -6444,21 +6444,21 @@
         <v>180</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -6466,10 +6466,10 @@
         <v>265</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -6480,7 +6480,7 @@
         <v>121</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -6488,10 +6488,10 @@
         <v>28</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -6499,10 +6499,10 @@
         <v>200</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
@@ -6510,10 +6510,10 @@
         <v>178</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -6521,10 +6521,10 @@
         <v>215</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -6532,10 +6532,10 @@
         <v>316</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -6543,10 +6543,10 @@
         <v>140</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -6554,10 +6554,10 @@
         <v>140</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -6565,10 +6565,10 @@
         <v>213</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
@@ -6576,21 +6576,21 @@
         <v>301</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -6598,10 +6598,10 @@
         <v>134</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -6609,10 +6609,10 @@
         <v>153</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -6620,10 +6620,10 @@
         <v>171</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -6631,10 +6631,10 @@
         <v>247</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -6642,21 +6642,21 @@
         <v>159</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -6664,10 +6664,10 @@
         <v>321</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -6675,10 +6675,10 @@
         <v>348</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -6689,7 +6689,7 @@
         <v>111</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -6697,21 +6697,21 @@
         <v>75</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -6719,10 +6719,10 @@
         <v>315</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -6730,10 +6730,10 @@
         <v>151</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -6741,10 +6741,10 @@
         <v>369</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -6752,10 +6752,10 @@
         <v>138</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>371</v>
+        <v>745</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>